<commit_message>
NO PUEDO CONESTO AUIDA
</commit_message>
<xml_diff>
--- a/python shenanigans/materias.xlsx
+++ b/python shenanigans/materias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\U\Season 7\Interacción Sociotécnologica\final\STI_Final\python shenanigans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{240C7C2A-0205-4CD7-ADFF-75C6E28BE87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98D0C09-79BD-43C5-9680-E22685422E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BFA4474-9CB8-4958-B0AC-2AB70BD3965A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="31">
   <si>
     <t>class_name</t>
   </si>
@@ -112,14 +112,37 @@
   </si>
   <si>
     <t>miercoles</t>
+  </si>
+  <si>
+    <t>classification</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>developer</t>
+  </si>
+  <si>
+    <t>UX</t>
+  </si>
+  <si>
+    <t>UI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -147,8 +170,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{058F30EC-CD21-40F8-86A4-7859B5A7F26F}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +498,7 @@
     <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,8 +508,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -495,8 +522,11 @@
       <c r="C2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -506,8 +536,11 @@
       <c r="C3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -517,8 +550,11 @@
       <c r="C4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -528,8 +564,11 @@
       <c r="C5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -539,8 +578,11 @@
       <c r="C6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -550,8 +592,11 @@
       <c r="C7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -561,8 +606,11 @@
       <c r="C8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -572,8 +620,11 @@
       <c r="C9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -583,8 +634,11 @@
       <c r="C10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -594,8 +648,11 @@
       <c r="C11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -605,8 +662,12 @@
       <c r="C12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -616,8 +677,11 @@
       <c r="C13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -627,8 +691,11 @@
       <c r="C14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -638,8 +705,11 @@
       <c r="C15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -649,8 +719,11 @@
       <c r="C16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -660,8 +733,11 @@
       <c r="C17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -671,8 +747,11 @@
       <c r="C18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -682,8 +761,12 @@
       <c r="C19" t="s">
         <v>22</v>
       </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>